<commit_message>
Week 6 (2 of 3 completed)
</commit_message>
<xml_diff>
--- a/Neeraj/Coursera/AlgorithmicToolbox/Rough_Explanation.xlsx
+++ b/Neeraj/Coursera/AlgorithmicToolbox/Rough_Explanation.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - leverage proactive deliverables\Java\JavaProjects\FAANGJobPreperation\Neeraj\Coursera\AlgorithmicToolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A799FAD-9149-48F4-848E-4E4DBB966667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1B697-D90A-492C-9E4D-DA079D33C30D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="3" xr2:uid="{19C6E116-7FAF-4ECE-98AF-7E930C9AD623}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{19C6E116-7FAF-4ECE-98AF-7E930C9AD623}"/>
   </bookViews>
   <sheets>
     <sheet name="W5.Coin Change" sheetId="2" r:id="rId1"/>
     <sheet name="W5.Primitive Calculator" sheetId="3" r:id="rId2"/>
     <sheet name="W5.Edit Distance" sheetId="1" r:id="rId3"/>
     <sheet name="W5.LongestCommonSubsequenceof2" sheetId="4" r:id="rId4"/>
+    <sheet name="W6" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,493 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neeraj Kumar singh</author>
+  </authors>
+  <commentList>
+    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{FF522559-15C9-4D45-A897-5B9AF7246617}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of 5-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{617EC52E-B106-4D3A-A9A9-D619E1EC95ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of below:
+m[1,1]-m[3,2] = (5-15)
+or
+m[2,1]-m[3,3] = (-3+7)
+or
+M[1,1]-M[3,2] = (5-15)
+or
+M[2,1]-M[3,3] = (-3+7)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{7F486AB4-8D94-41DD-99B8-3F15997AD3B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope: (5-8+7*4)
+T[4,1]=
+Min of:
+T[], ie -3+28 or
+T[], ie -10*4 or
+T[], ie 4*4 or
+T[], ie 5-60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE4" authorId="0" shapeId="0" xr:uid="{1DCD80A4-8D8B-40AA-83F4-77F719C88C8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Max of below:
+m[1,1]-m[3,2] = (5-15)
+or
+m[2,1]-m[3,3] = (-3+7)
+or
+M[1,1]-M[3,2] = (5-15)
+or
+M[2,1]-M[3,3] = (-3+7)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF4" authorId="0" shapeId="0" xr:uid="{036FC634-FA82-4665-87D1-8208D51E87CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope: (5-8+7*4)
+Max of:
+-3+28 or
+-10*4 or
+4*4 or
+5-60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X5" authorId="0" shapeId="0" xr:uid="{531A98A7-8A87-428C-B32F-2FAFD3BEF835}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of 8+7</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y5" authorId="0" shapeId="0" xr:uid="{7D75AC46-6C8A-4D54-AF7F-423118BABC90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of
+15*4 or
+8+28 or
+15*4 or
+8+28 or</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z5" authorId="0" shapeId="0" xr:uid="{96A2355B-8B75-4B8B-9F9D-7FEEACC48805}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope: (8+7*4-8)
+T[2,5]=
+Min of:
+m[2,2]+m[3,5], ie 8+(-28) or
+m[2,3]*m[4,5] , ie 15*(-4) or
+M[2,2]+M[3,5], ie 8+20 or
+M[2,3]*M[4,5] , ie 15*(-4)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF5" authorId="0" shapeId="0" xr:uid="{BDF0D2A6-82A5-4489-9BA5-CAC76812124F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Max of
+15*4 or
+8+28 or
+15*4 or
+8+28 or</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{2873A93F-6567-4C46-98FC-5AC5B3BE7F83}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope: (8+7*4-8)
+T[2,5]=
+Max of:
+m[2,2]+m[3,5], ie 8+(-28) or
+m[2,3]*m[4,5] , ie 15*(-4) or
+m[2,4]-m[5,5] , ie 36-8 or
+M[2,2]+M[3,5], ie 8+20 or
+M[2,3]*M[4,5] , ie 15*(-4) or
+M[2,4]-M[5,5] , ie 60-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{E6F29B9E-8194-40C7-B7A5-6C1F15192C4B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of 7*4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{3DF23C58-4FD0-4861-9E5F-CF5CA42B3EB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope (7*4-8)
+Min of
+7*(-4) or
+28-8 or
+7*(-4) or
+28-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG6" authorId="0" shapeId="0" xr:uid="{35AAC57B-EEB6-4D71-A5B3-445D5F188159}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In Scope (7*4-8)
+Max of
+7*(-4) or
+28-8 or
+7*(-4) or
+28-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z7" authorId="0" shapeId="0" xr:uid="{0FD7FFAB-B58A-4ED5-85F9-66D42DDD756A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of 4-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA7" authorId="0" shapeId="0" xr:uid="{1B6C6DDA-0467-4834-A324-77342B20C519}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Inscope: (4-8+9)
+Min of
+4-17 or
+-4+9 or
+4-17 or
+-4+9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH7" authorId="0" shapeId="0" xr:uid="{912B9C9B-DD7E-41FB-8C84-50317E084206}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Inscope: (4-8+9)
+Min of
+4-17 or
+-4+9 or
+4-17 or
+-4+9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA8" authorId="0" shapeId="0" xr:uid="{7ADF3C3B-D894-48F8-B2EA-55E188A73B24}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neeraj Kumar singh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Min of 8+9</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
   <si>
     <t>b</t>
   </si>
@@ -276,12 +762,72 @@
   <si>
     <t>Sample 3</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Maximum Amount of Gold</t>
+  </si>
+  <si>
+    <t>Partitioning Souvenirs</t>
+  </si>
+  <si>
+    <t>Sample 1:</t>
+  </si>
+  <si>
+    <t>Sum = 12</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Set to true as we can have partitions of zero.</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>3,3,3</t>
+  </si>
+  <si>
+    <t>3,3,3,3</t>
+  </si>
+  <si>
+    <t>And how check if the subset of J can be partitioned into value in I</t>
+  </si>
+  <si>
+    <t>Sample 3:</t>
+  </si>
+  <si>
+    <t>Maximum Value of an Arithmetic Expression</t>
+  </si>
+  <si>
+    <t>Sample 2:</t>
+  </si>
+  <si>
+    <t>5-8+7*4-8+9</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +865,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -359,7 +918,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -395,17 +954,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -413,9 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -468,6 +1041,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,7 +1835,7 @@
   <dimension ref="A1:AI4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,110 +1951,110 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>2</v>
-      </c>
-      <c r="D2" s="9">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9">
-        <v>5</v>
-      </c>
-      <c r="G2" s="9">
+    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>7</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="7">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="7">
         <v>9</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="7">
         <v>11</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="7">
         <v>12</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="7">
         <v>13</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="7">
         <v>14</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="7">
         <v>15</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="7">
         <v>16</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="7">
         <v>17</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="7">
         <v>18</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="7">
         <v>19</v>
       </c>
-      <c r="U2" s="9">
+      <c r="U2" s="7">
         <v>20</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="7">
         <v>21</v>
       </c>
-      <c r="W2" s="9">
+      <c r="W2" s="7">
         <v>22</v>
       </c>
-      <c r="X2" s="9">
+      <c r="X2" s="7">
         <v>23</v>
       </c>
-      <c r="Y2" s="9">
+      <c r="Y2" s="7">
         <v>24</v>
       </c>
-      <c r="Z2" s="9">
+      <c r="Z2" s="7">
         <v>25</v>
       </c>
-      <c r="AA2" s="9">
+      <c r="AA2" s="7">
         <v>26</v>
       </c>
-      <c r="AB2" s="9">
+      <c r="AB2" s="7">
         <v>27</v>
       </c>
-      <c r="AC2" s="9">
+      <c r="AC2" s="7">
         <v>28</v>
       </c>
-      <c r="AD2" s="9">
+      <c r="AD2" s="7">
         <v>29</v>
       </c>
-      <c r="AE2" s="9">
+      <c r="AE2" s="7">
         <v>30</v>
       </c>
-      <c r="AF2" s="9">
+      <c r="AF2" s="7">
         <v>31</v>
       </c>
-      <c r="AG2" s="9">
+      <c r="AG2" s="7">
         <v>32</v>
       </c>
-      <c r="AH2" s="9">
+      <c r="AH2" s="7">
         <v>33</v>
       </c>
-      <c r="AI2" s="9">
+      <c r="AI2" s="7">
         <v>34</v>
       </c>
     </row>
@@ -1574,104 +2165,104 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9">
-        <v>2</v>
-      </c>
-      <c r="G4" s="9">
-        <v>3</v>
-      </c>
-      <c r="H4" s="9">
-        <v>2</v>
-      </c>
-      <c r="I4" s="9">
-        <v>2</v>
-      </c>
-      <c r="J4" s="9">
-        <v>3</v>
-      </c>
-      <c r="K4" s="9">
-        <v>3</v>
-      </c>
-      <c r="L4" s="9">
-        <v>3</v>
-      </c>
-      <c r="M4" s="9">
-        <v>3</v>
-      </c>
-      <c r="N4" s="9">
-        <v>4</v>
-      </c>
-      <c r="O4" s="9">
-        <v>4</v>
-      </c>
-      <c r="P4" s="9">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>4</v>
-      </c>
-      <c r="R4" s="9">
-        <v>5</v>
-      </c>
-      <c r="S4" s="9">
-        <v>5</v>
-      </c>
-      <c r="T4" s="9">
-        <v>5</v>
-      </c>
-      <c r="U4" s="9">
-        <v>5</v>
-      </c>
-      <c r="V4" s="9">
+    <row r="4" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3</v>
+      </c>
+      <c r="L4" s="7">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7">
+        <v>3</v>
+      </c>
+      <c r="N4" s="7">
+        <v>4</v>
+      </c>
+      <c r="O4" s="7">
+        <v>4</v>
+      </c>
+      <c r="P4" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4</v>
+      </c>
+      <c r="R4" s="7">
+        <v>5</v>
+      </c>
+      <c r="S4" s="7">
+        <v>5</v>
+      </c>
+      <c r="T4" s="7">
+        <v>5</v>
+      </c>
+      <c r="U4" s="7">
+        <v>5</v>
+      </c>
+      <c r="V4" s="7">
         <v>6</v>
       </c>
-      <c r="W4" s="9">
+      <c r="W4" s="7">
         <v>6</v>
       </c>
-      <c r="X4" s="9">
+      <c r="X4" s="7">
         <v>6</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="Y4" s="7">
         <v>6</v>
       </c>
-      <c r="Z4" s="9">
+      <c r="Z4" s="7">
         <v>7</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="7">
         <v>7</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AB4" s="7">
         <v>7</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AC4" s="7">
         <v>7</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF4" s="7">
         <v>8</v>
       </c>
-      <c r="AG4" s="9">
+      <c r="AG4" s="7">
         <v>7</v>
       </c>
-      <c r="AH4" s="9">
+      <c r="AH4" s="7">
         <v>9</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AI4" s="7">
         <v>9</v>
       </c>
     </row>
@@ -1688,7 +2279,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,56 +2299,56 @@
     <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="S1"/>
@@ -1768,361 +2359,361 @@
       <c r="X1"/>
       <c r="Y1"/>
     </row>
-    <row r="2" spans="1:25" s="17" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:25" s="15" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <f>LEN(B3)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>LEN(C3)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="14">
         <f t="shared" ref="D2:J2" si="0">LEN(D3)</f>
         <v>2</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="14">
         <f t="shared" ref="K2" si="1">LEN(K3)</f>
         <v>9</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="14">
         <f t="shared" ref="L2" si="2">LEN(L3)</f>
         <v>10</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="14">
         <f t="shared" ref="M2" si="3">LEN(M3)</f>
         <v>11</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="14">
         <f t="shared" ref="N2" si="4">LEN(N3)</f>
         <v>12</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="14">
         <f t="shared" ref="O2" si="5">LEN(O3)</f>
         <v>13</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="14">
         <f t="shared" ref="P2:Q2" si="6">LEN(P3)</f>
         <v>14</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="14">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
         <v>11</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>111</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>1111</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <v>11111</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>111111</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="11">
         <v>1111111</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="11">
         <v>11111111</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="11">
         <v>111111111</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="11">
         <v>1111111111</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="26" t="s">
+      <c r="O3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:25" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <f>LEN(B5)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <f t="shared" ref="C4:J4" si="7">LEN(C5)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="16">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="16">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="16">
         <f t="shared" ref="K4" si="8">LEN(K5)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="16">
         <f t="shared" ref="L4" si="9">LEN(L5)</f>
         <v>5</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="16">
         <f t="shared" ref="M4" si="10">LEN(M5)</f>
         <v>4</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="16">
         <f t="shared" ref="N4" si="11">LEN(N5)</f>
         <v>5</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="16">
         <f t="shared" ref="O4" si="12">LEN(O5)</f>
         <v>5</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="16">
         <f t="shared" ref="P4:Q4" si="13">LEN(P5)</f>
         <v>6</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12">
         <v>21</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>22</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>221</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>212</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>2121</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <v>222</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>2221</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="12">
         <v>2212</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <v>22121</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="12">
         <v>2122</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>21221</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="12">
         <v>21212</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="12">
         <v>212121</v>
       </c>
-      <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="1:25" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="23" t="s">
+      <c r="Q5" s="12"/>
+    </row>
+    <row r="6" spans="1:25" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.5">
+      <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <f>LEN(B7)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="18">
         <f t="shared" ref="C6:J6" si="14">LEN(C7)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="18">
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="18">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="18">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="18">
         <f t="shared" ref="K6" si="15">LEN(K7)</f>
         <v>3</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="18">
         <f t="shared" ref="L6" si="16">LEN(L7)</f>
         <v>4</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="18">
         <f t="shared" ref="M6" si="17">LEN(M7)</f>
         <v>3</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="18">
         <f t="shared" ref="N6" si="18">LEN(N7)</f>
         <v>4</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="18">
         <f t="shared" ref="O6" si="19">LEN(O7)</f>
         <v>4</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="18">
         <f t="shared" ref="P6:Q6" si="20">LEN(P7)</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="18">
         <f t="shared" si="20"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15">
-        <v>2</v>
-      </c>
-      <c r="D7" s="15">
-        <v>3</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
         <v>31</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>311</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>32</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <v>321</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <v>3211</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="13">
         <v>33</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="13">
         <v>331</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="13">
         <v>3311</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="13">
         <v>322</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="13">
         <v>3221</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="13">
         <v>3212</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="13">
         <v>3113</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="23">
         <v>32112</v>
       </c>
     </row>
@@ -2154,47 +2745,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6">
+      <c r="A1" s="28">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="7" t="s">
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5">
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="1">
@@ -2209,27 +2800,27 @@
       <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>0</v>
       </c>
-      <c r="N2" s="8">
-        <v>1</v>
-      </c>
-      <c r="O2" s="8">
-        <v>2</v>
-      </c>
-      <c r="P2" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>4</v>
-      </c>
-      <c r="R2" s="8">
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
+        <v>2</v>
+      </c>
+      <c r="P2" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>4</v>
+      </c>
+      <c r="R2" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -2238,7 +2829,7 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="1">
@@ -2250,30 +2841,30 @@
       <c r="G3" s="1">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>55</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="29">
-        <v>1</v>
-      </c>
-      <c r="O3" s="29">
-        <v>2</v>
-      </c>
-      <c r="P3" s="29">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="29">
-        <v>4</v>
-      </c>
-      <c r="R3" s="29">
+      <c r="N3" s="27">
+        <v>1</v>
+      </c>
+      <c r="O3" s="27">
+        <v>2</v>
+      </c>
+      <c r="P3" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>4</v>
+      </c>
+      <c r="R3" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -2285,7 +2876,7 @@
       <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1</v>
       </c>
       <c r="F4" s="1">
@@ -2294,30 +2885,30 @@
       <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
-      <c r="N4" s="29">
-        <v>2</v>
-      </c>
-      <c r="O4" s="29">
-        <v>2</v>
-      </c>
-      <c r="P4" s="29">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="29">
-        <v>3</v>
-      </c>
-      <c r="R4" s="29">
+      <c r="N4" s="27">
+        <v>2</v>
+      </c>
+      <c r="O4" s="27">
+        <v>2</v>
+      </c>
+      <c r="P4" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="27">
+        <v>3</v>
+      </c>
+      <c r="R4" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -2332,36 +2923,36 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M5">
         <v>3</v>
       </c>
-      <c r="N5" s="29">
-        <v>3</v>
-      </c>
-      <c r="O5" s="29">
-        <v>3</v>
-      </c>
-      <c r="P5" s="29">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="29">
-        <v>2</v>
-      </c>
-      <c r="R5" s="29">
+      <c r="N5" s="27">
+        <v>3</v>
+      </c>
+      <c r="O5" s="27">
+        <v>3</v>
+      </c>
+      <c r="P5" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>2</v>
+      </c>
+      <c r="R5" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -2376,36 +2967,36 @@
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>2</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="M6">
         <v>4</v>
       </c>
-      <c r="N6" s="29">
-        <v>4</v>
-      </c>
-      <c r="O6" s="29">
-        <v>4</v>
-      </c>
-      <c r="P6" s="29">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>3</v>
-      </c>
-      <c r="R6" s="29">
+      <c r="N6" s="27">
+        <v>4</v>
+      </c>
+      <c r="O6" s="27">
+        <v>4</v>
+      </c>
+      <c r="P6" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="27">
+        <v>3</v>
+      </c>
+      <c r="R6" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -2420,36 +3011,36 @@
       <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>51</v>
       </c>
       <c r="M7">
         <v>5</v>
       </c>
-      <c r="N7" s="29">
-        <v>4</v>
-      </c>
-      <c r="O7" s="29">
-        <v>5</v>
-      </c>
-      <c r="P7" s="29">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>4</v>
-      </c>
-      <c r="R7" s="29">
+      <c r="N7" s="27">
+        <v>4</v>
+      </c>
+      <c r="O7" s="27">
+        <v>5</v>
+      </c>
+      <c r="P7" s="27">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>4</v>
+      </c>
+      <c r="R7" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -2467,16 +3058,16 @@
       <c r="F8" s="1">
         <v>4</v>
       </c>
-      <c r="G8" s="5">
-        <v>4</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2491,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E30AD1-1F61-49BB-BE2C-9FC66170F84A}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2565,13 +3156,13 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="15">
-        <v>1</v>
-      </c>
-      <c r="D3" s="15">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
         <v>1</v>
       </c>
       <c r="H3">
@@ -2580,16 +3171,16 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="13">
         <v>0</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="13">
         <v>0</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="13">
         <v>0</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2600,13 +3191,13 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="15">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15">
-        <v>1</v>
-      </c>
-      <c r="E4" s="15">
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
         <v>2</v>
       </c>
       <c r="H4">
@@ -2615,16 +3206,16 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4" s="15">
-        <v>1</v>
-      </c>
-      <c r="K4" s="15">
-        <v>1</v>
-      </c>
-      <c r="L4" s="15">
-        <v>1</v>
-      </c>
-      <c r="M4" s="15">
+      <c r="J4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2635,43 +3226,43 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" s="15">
-        <v>1</v>
-      </c>
-      <c r="K5" s="15">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15">
-        <v>2</v>
-      </c>
-      <c r="M5" s="15">
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1</v>
+      </c>
+      <c r="L5" s="13">
+        <v>2</v>
+      </c>
+      <c r="M5" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="H6">
         <v>7</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6" s="15">
-        <v>1</v>
-      </c>
-      <c r="K6" s="15">
-        <v>2</v>
-      </c>
-      <c r="L6" s="15">
-        <v>2</v>
-      </c>
-      <c r="M6" s="15">
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13">
+        <v>2</v>
+      </c>
+      <c r="L6" s="13">
+        <v>2</v>
+      </c>
+      <c r="M6" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2682,4 +3273,585 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D48B82-BC3B-4040-94F0-EE673E58B6EB}">
+  <dimension ref="A1:AH19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AA21" sqref="AA21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="B1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="U1" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="30">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2" s="30">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="U2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="30">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="30">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" s="30">
+        <v>4</v>
+      </c>
+      <c r="B4" s="30">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30">
+        <v>1</v>
+      </c>
+      <c r="E4" s="30">
+        <v>4</v>
+      </c>
+      <c r="F4" s="30">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30">
+        <v>5</v>
+      </c>
+      <c r="H4" s="30">
+        <v>5</v>
+      </c>
+      <c r="I4" s="30">
+        <v>5</v>
+      </c>
+      <c r="J4" s="30">
+        <v>5</v>
+      </c>
+      <c r="K4" s="30">
+        <v>5</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="31">
+        <v>5</v>
+      </c>
+      <c r="W4" s="31">
+        <v>-3</v>
+      </c>
+      <c r="X4" s="31">
+        <v>-10</v>
+      </c>
+      <c r="Y4" s="31">
+        <v>-55</v>
+      </c>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AC4" s="31">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="31">
+        <v>-3</v>
+      </c>
+      <c r="AE4" s="31">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="31">
+        <v>25</v>
+      </c>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="30">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" s="30">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31">
+        <v>8</v>
+      </c>
+      <c r="X5" s="31">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="31">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="31">
+        <v>-60</v>
+      </c>
+      <c r="AA5" s="31"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="31">
+        <v>8</v>
+      </c>
+      <c r="AE5" s="31">
+        <v>15</v>
+      </c>
+      <c r="AF5" s="31">
+        <v>60</v>
+      </c>
+      <c r="AG5" s="31">
+        <v>52</v>
+      </c>
+      <c r="AH5" s="31"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="31">
+        <v>28</v>
+      </c>
+      <c r="Z6" s="31">
+        <v>-28</v>
+      </c>
+      <c r="AA6" s="31"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="31"/>
+      <c r="AE6" s="31">
+        <v>7</v>
+      </c>
+      <c r="AF6" s="31">
+        <v>28</v>
+      </c>
+      <c r="AG6" s="31">
+        <v>20</v>
+      </c>
+      <c r="AH6" s="31"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="31">
+        <v>-4</v>
+      </c>
+      <c r="AA7" s="31">
+        <v>-13</v>
+      </c>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="31">
+        <v>4</v>
+      </c>
+      <c r="AG7" s="31">
+        <v>-4</v>
+      </c>
+      <c r="AH7" s="31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C8" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="31">
+        <v>17</v>
+      </c>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+      <c r="AG8" s="31">
+        <v>8</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="31">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="31"/>
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="31"/>
+      <c r="AG9" s="31"/>
+      <c r="AH9" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="35">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="35">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" t="s">
+        <v>72</v>
+      </c>
+      <c r="W11" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="X11" s="34"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AD11" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE11" s="34"/>
+      <c r="AF11" s="34"/>
+      <c r="AG11" s="34"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>59</v>
+      </c>
+      <c r="G18">
+        <v>34</v>
+      </c>
+      <c r="H18">
+        <v>57</v>
+      </c>
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <v>23</v>
+      </c>
+      <c r="K18">
+        <v>67</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>18</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="W11:Z11"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="U1:AE1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>